<commit_message>
Newest version of master timesheet. Recorded work time for meeting held on 10/8/2024.
</commit_message>
<xml_diff>
--- a/CEN3907C Effort Log.xlsx
+++ b/CEN3907C Effort Log.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Sheet4" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Joshua" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Tyler" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Augustus" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Andrew" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Sheet5" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
@@ -20,6 +20,12 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C4">
+      <text>
+        <t xml:space="preserve">Design Draft Finalization and Meeting
+	-Joshua</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="B4">
       <text>
         <t xml:space="preserve">Work on Design Draft
@@ -38,6 +44,46 @@
       <text>
         <t xml:space="preserve">Meeting + Research
 	-Joshua</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B4">
+      <text>
+        <t xml:space="preserve">We discussed each others progress on the parts of the design draft and gave each other feedback about the parts we have done
+	-Andrew Miller</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H2">
+      <text>
+        <t xml:space="preserve">I first spent sometime researching the various microchips we could possibly use. We decided it would either be a DW3000 or a RFID chip so I did some research on the DW3000 since that is the idea we are going with for now. Then I spent time finding the pin layouts for the two chip componts that will be in the football the DW3000 and the nRF52 and did the draft schematic and told how we would connect them for SPI use.
+	-Andrew Miller</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E2">
+      <text>
+        <t xml:space="preserve">We made changes to our design and switched which type of microcontroller would be sending and receiving data from the football
+	-Andrew Miller</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D2">
+      <text>
+        <t xml:space="preserve">I was working on the draft schematic for the design draft so I spent my time researching how all our hardware was communicating and then I created a first draft of the draft schematic and put it in the document
+	-Andrew Miller</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C2">
+      <text>
+        <t xml:space="preserve">Today we had our first meeting where we discussed the project and started working on the design draft.
+	-Andrew Miller</t>
       </text>
     </comment>
   </commentList>
@@ -530,7 +576,7 @@
       </c>
       <c r="M2" s="6">
         <f>SUM(I2:I52)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -564,7 +610,9 @@
       <c r="B4" s="5">
         <v>2.0</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5">
+        <v>2.0</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -572,7 +620,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f>SUM(B4:H4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1586,20 +1634,30 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="B2" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.0</v>
+      </c>
       <c r="I2" s="6">
         <f>SUM(B2:H2)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M2" s="6">
         <f>SUM(I2:I52)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -1630,8 +1688,12 @@
     </row>
     <row r="4">
       <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.0</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1639,7 +1701,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f>SUM(B4:H4)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -2606,6 +2668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2653,19 +2716,23 @@
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2.0</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="6">
         <f>SUM(B2:H2)</f>
-        <v>0</v>
+        <v>3.92</v>
       </c>
       <c r="M2" s="6">
         <f>SUM(I2:I52)</f>
-        <v>0</v>
+        <v>6.92</v>
       </c>
     </row>
     <row r="3">
@@ -2696,8 +2763,12 @@
     </row>
     <row r="4">
       <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.0</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -2705,7 +2776,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f>SUM(B4:H4)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -3664,6 +3735,9 @@
       <c r="A53" s="9"/>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3719,19 +3793,27 @@
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2.0</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5">
+        <v>2.0</v>
+      </c>
       <c r="I2" s="6">
         <f>SUM(B2:H2)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M2" s="6">
         <f>SUM(I2:I52)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -3762,7 +3844,9 @@
     </row>
     <row r="4">
       <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5">
+        <v>1.0</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3771,7 +3855,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f>SUM(B4:H4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -4730,7 +4814,8 @@
       <c r="A53" s="9"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>